<commit_message>
added defect image for Zachary
</commit_message>
<xml_diff>
--- a/Data/Dataset-1b/labels_updated.xlsx
+++ b/Data/Dataset-1b/labels_updated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/36cfa90f76623f7a/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanzhouf\Documents\GitHub\Dataset-in-situ-monitoring-FFF-structures\Data\Dataset-1b\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="553" documentId="8_{3546AF54-BBA6-4BE7-BF5B-171329BBE1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3F68919-ED35-4669-A920-8118474146D2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A20F2DD-7897-4ECE-849C-D17D907EF1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="3312" windowWidth="17280" windowHeight="8880" xr2:uid="{EA8A39CE-B19A-4A99-8F89-EE0F26CEA7D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{EA8A39CE-B19A-4A99-8F89-EE0F26CEA7D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -586,12 +586,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -908,13 +909,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD83569-EED5-4AD4-82B2-CEFE13CFF871}">
   <dimension ref="A1:AJ535"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="F151" sqref="F151"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="E143" sqref="E143:K143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -964,7 +965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1014,7 +1015,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1064,7 +1065,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1114,7 +1115,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1164,7 +1165,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1214,7 +1215,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1264,7 +1265,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1314,7 +1315,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1364,7 +1365,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1414,7 +1415,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1464,7 +1465,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1514,7 +1515,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1564,7 +1565,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1614,7 +1615,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1664,7 +1665,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1714,7 +1715,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1764,7 +1765,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1814,7 +1815,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1864,7 +1865,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1914,7 +1915,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1964,7 +1965,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2014,7 +2015,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2064,7 +2065,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2114,7 +2115,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2164,7 +2165,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2214,7 +2215,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2264,7 +2265,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2314,7 +2315,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2364,7 +2365,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2414,7 +2415,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2464,7 +2465,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2514,7 +2515,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2564,7 +2565,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2614,7 +2615,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2664,7 +2665,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2714,7 +2715,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2764,7 +2765,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2814,7 +2815,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2864,7 +2865,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2914,7 +2915,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2964,7 +2965,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3014,7 +3015,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3064,7 +3065,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3114,7 +3115,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3164,7 +3165,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3214,7 +3215,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3264,7 +3265,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3314,7 +3315,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3409,7 +3410,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3504,7 +3505,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3599,7 +3600,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3649,7 +3650,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3699,7 +3700,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3749,7 +3750,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3799,7 +3800,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3894,7 +3895,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3989,7 +3990,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -4084,7 +4085,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -4134,7 +4135,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -4184,7 +4185,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -4234,7 +4235,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -4284,7 +4285,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -4334,7 +4335,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -4384,7 +4385,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -4434,7 +4435,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -4484,7 +4485,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -4534,7 +4535,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -4584,7 +4585,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -4634,7 +4635,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -4684,7 +4685,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4734,7 +4735,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -4784,7 +4785,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -4834,7 +4835,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -4884,7 +4885,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -4934,7 +4935,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -4984,7 +4985,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -5034,7 +5035,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -5084,7 +5085,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -5134,7 +5135,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -5184,7 +5185,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -5234,7 +5235,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -5284,7 +5285,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -5334,7 +5335,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -5384,7 +5385,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -5434,7 +5435,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -5484,7 +5485,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -5534,7 +5535,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -5584,7 +5585,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -5634,7 +5635,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -5684,7 +5685,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -5734,7 +5735,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -5747,25 +5748,25 @@
       <c r="D92">
         <v>5</v>
       </c>
-      <c r="E92" s="2">
-        <v>2</v>
-      </c>
-      <c r="F92" s="2">
+      <c r="E92" s="3">
+        <v>2</v>
+      </c>
+      <c r="F92" s="3">
         <v>7.5</v>
       </c>
-      <c r="G92" s="2">
-        <v>2</v>
-      </c>
-      <c r="H92" s="2">
+      <c r="G92" s="3">
+        <v>2</v>
+      </c>
+      <c r="H92" s="3">
         <v>5</v>
       </c>
-      <c r="I92" s="2">
-        <v>2</v>
-      </c>
-      <c r="J92" s="2">
+      <c r="I92" s="3">
+        <v>2</v>
+      </c>
+      <c r="J92" s="3">
         <v>7.5</v>
       </c>
-      <c r="K92" s="2">
+      <c r="K92" s="3">
         <v>3</v>
       </c>
       <c r="L92">
@@ -5784,7 +5785,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -5834,7 +5835,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -5884,7 +5885,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -5934,7 +5935,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -5984,7 +5985,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -6034,7 +6035,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -6084,7 +6085,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -6134,7 +6135,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -6184,7 +6185,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -6234,7 +6235,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -6284,7 +6285,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -6334,7 +6335,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -6384,7 +6385,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -6434,7 +6435,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -6484,7 +6485,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -6534,7 +6535,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -6584,7 +6585,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -6634,7 +6635,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -6684,7 +6685,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -6734,7 +6735,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -6784,7 +6785,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -6834,7 +6835,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -6884,7 +6885,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -6934,7 +6935,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -6984,7 +6985,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -7034,7 +7035,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -7084,7 +7085,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -7134,7 +7135,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -7184,7 +7185,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -7234,7 +7235,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -7284,7 +7285,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -7334,7 +7335,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -7384,7 +7385,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -7434,7 +7435,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -7484,7 +7485,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -7534,7 +7535,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -7584,7 +7585,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -7634,7 +7635,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -7684,7 +7685,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -7734,7 +7735,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -7784,7 +7785,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -7834,7 +7835,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -7884,7 +7885,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -7934,7 +7935,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -7984,7 +7985,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -8034,7 +8035,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -8084,7 +8085,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -8134,7 +8135,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -8184,7 +8185,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -8234,7 +8235,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -8284,7 +8285,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -8297,25 +8298,25 @@
       <c r="D143">
         <v>5</v>
       </c>
-      <c r="E143" s="2">
-        <v>3</v>
-      </c>
-      <c r="F143" s="2">
+      <c r="E143" s="3">
+        <v>3</v>
+      </c>
+      <c r="F143" s="3">
         <v>7.5</v>
       </c>
-      <c r="G143" s="2">
-        <v>2</v>
-      </c>
-      <c r="H143" s="2">
+      <c r="G143" s="3">
+        <v>2</v>
+      </c>
+      <c r="H143" s="3">
         <v>5</v>
       </c>
-      <c r="I143" s="2">
-        <v>3</v>
-      </c>
-      <c r="J143" s="2">
+      <c r="I143" s="3">
+        <v>3</v>
+      </c>
+      <c r="J143" s="3">
         <v>7.5</v>
       </c>
-      <c r="K143" s="2">
+      <c r="K143" s="3">
         <v>3</v>
       </c>
       <c r="L143">
@@ -8334,7 +8335,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -8384,7 +8385,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -8434,7 +8435,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -8484,7 +8485,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -8534,7 +8535,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -8584,7 +8585,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -8634,7 +8635,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -8684,7 +8685,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -8734,7 +8735,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -8784,7 +8785,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -8834,7 +8835,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -8884,1907 +8885,1907 @@
         <v>74</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>300</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>304</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>305</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>306</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>307</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>308</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>309</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>310</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>311</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>312</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>313</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>314</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>315</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>316</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>317</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>318</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>319</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>320</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>321</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>322</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>323</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>324</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>325</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>326</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>327</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>328</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>329</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>330</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>331</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>332</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>333</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>334</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>335</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>336</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>337</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>338</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>339</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>340</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>341</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>342</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>343</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>344</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>345</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>346</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>347</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>348</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>349</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>350</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>351</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>352</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>353</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <v>354</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <v>355</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <v>356</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
         <v>357</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
         <v>358</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>359</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <v>360</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <v>361</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <v>362</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>363</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <v>364</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>365</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
         <v>366</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="1">
         <v>367</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A369" s="1">
         <v>368</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
         <v>369</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" s="1">
         <v>370</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
         <v>371</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
         <v>372</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" s="1">
         <v>373</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" s="1">
         <v>374</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" s="1">
         <v>375</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" s="1">
         <v>376</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" s="1">
         <v>377</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" s="1">
         <v>378</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" s="1">
         <v>379</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" s="1">
         <v>380</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" s="1">
         <v>381</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" s="1">
         <v>382</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" s="1">
         <v>383</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="1">
         <v>384</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" s="1">
         <v>385</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
         <v>386</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388" s="1">
         <v>387</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" s="1">
         <v>388</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A390" s="1">
         <v>389</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" s="1">
         <v>390</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
         <v>391</v>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" s="1">
         <v>392</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A394" s="1">
         <v>393</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
         <v>394</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
         <v>395</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
         <v>396</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
         <v>397</v>
       </c>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" s="1">
         <v>398</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A400" s="1">
         <v>399</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A401" s="1">
         <v>400</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
         <v>401</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A403" s="1">
         <v>402</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
         <v>403</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
         <v>404</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
         <v>405</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
         <v>406</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A408" s="1">
         <v>407</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" s="1">
         <v>408</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A410" s="1">
         <v>409</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A411" s="1">
         <v>410</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A412" s="1">
         <v>411</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A413" s="1">
         <v>412</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A414" s="1">
         <v>413</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" s="1">
         <v>414</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A416" s="1">
         <v>415</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A417" s="1">
         <v>416</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
         <v>417</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A419" s="1">
         <v>418</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" s="1">
         <v>419</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
         <v>420</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
         <v>421</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A423" s="1">
         <v>422</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A424" s="1">
         <v>423</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A425" s="1">
         <v>424</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A426" s="1">
         <v>425</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" s="1">
         <v>426</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A428" s="1">
         <v>427</v>
       </c>
     </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" s="1">
         <v>428</v>
       </c>
     </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A430" s="1">
         <v>429</v>
       </c>
     </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A431" s="1">
         <v>430</v>
       </c>
     </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A432" s="1">
         <v>431</v>
       </c>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A433" s="1">
         <v>432</v>
       </c>
     </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A434" s="1">
         <v>433</v>
       </c>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A435" s="1">
         <v>434</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A436" s="1">
         <v>435</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" s="1">
         <v>436</v>
       </c>
     </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A438" s="1">
         <v>437</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" s="1">
         <v>438</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A440" s="1">
         <v>439</v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A441" s="1">
         <v>440</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
         <v>441</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A443" s="1">
         <v>442</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A444" s="1">
         <v>443</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A445" s="1">
         <v>444</v>
       </c>
     </row>
-    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A446" s="1">
         <v>445</v>
       </c>
     </row>
-    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447" s="1">
         <v>446</v>
       </c>
     </row>
-    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A448" s="1">
         <v>447</v>
       </c>
     </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A449" s="1">
         <v>448</v>
       </c>
     </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A450" s="1">
         <v>449</v>
       </c>
     </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A451" s="1">
         <v>450</v>
       </c>
     </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A452" s="1">
         <v>451</v>
       </c>
     </row>
-    <row r="453" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453" s="1">
         <v>452</v>
       </c>
     </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A454" s="1">
         <v>453</v>
       </c>
     </row>
-    <row r="455" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" s="1">
         <v>454</v>
       </c>
     </row>
-    <row r="456" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A456" s="1">
         <v>455</v>
       </c>
     </row>
-    <row r="457" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A457" s="1">
         <v>456</v>
       </c>
     </row>
-    <row r="458" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A458" s="1">
         <v>457</v>
       </c>
     </row>
-    <row r="459" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" s="1">
         <v>458</v>
       </c>
     </row>
-    <row r="460" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A460" s="1">
         <v>459</v>
       </c>
     </row>
-    <row r="461" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" s="1">
         <v>460</v>
       </c>
     </row>
-    <row r="462" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A462" s="1">
         <v>461</v>
       </c>
     </row>
-    <row r="463" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A463" s="1">
         <v>462</v>
       </c>
     </row>
-    <row r="464" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" s="1">
         <v>463</v>
       </c>
     </row>
-    <row r="465" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A465" s="1">
         <v>464</v>
       </c>
     </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A466" s="1">
         <v>465</v>
       </c>
     </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A467" s="1">
         <v>466</v>
       </c>
     </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468" s="1">
         <v>467</v>
       </c>
     </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A469" s="1">
         <v>468</v>
       </c>
     </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A470" s="1">
         <v>469</v>
       </c>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" s="1">
         <v>470</v>
       </c>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A472" s="1">
         <v>471</v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A473" s="1">
         <v>472</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A474" s="1">
         <v>473</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A475" s="1">
         <v>474</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A476" s="1">
         <v>475</v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A477" s="1">
         <v>476</v>
       </c>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A478" s="1">
         <v>477</v>
       </c>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A479" s="1">
         <v>478</v>
       </c>
     </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A480" s="1">
         <v>479</v>
       </c>
     </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A481" s="1">
         <v>480</v>
       </c>
     </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482" s="1">
         <v>481</v>
       </c>
     </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A483" s="1">
         <v>482</v>
       </c>
     </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A484" s="1">
         <v>483</v>
       </c>
     </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A485" s="1">
         <v>484</v>
       </c>
     </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A486" s="1">
         <v>485</v>
       </c>
     </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A487" s="1">
         <v>486</v>
       </c>
     </row>
-    <row r="488" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A488" s="1">
         <v>487</v>
       </c>
     </row>
-    <row r="489" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" s="1">
         <v>488</v>
       </c>
     </row>
-    <row r="490" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A490" s="1">
         <v>489</v>
       </c>
     </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" s="1">
         <v>490</v>
       </c>
     </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" s="1">
         <v>491</v>
       </c>
     </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A493" s="1">
         <v>492</v>
       </c>
     </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A494" s="1">
         <v>493</v>
       </c>
     </row>
-    <row r="495" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A495" s="1">
         <v>494</v>
       </c>
     </row>
-    <row r="496" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A496" s="1">
         <v>495</v>
       </c>
     </row>
-    <row r="497" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A497" s="1">
         <v>496</v>
       </c>
     </row>
-    <row r="498" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A498" s="1">
         <v>497</v>
       </c>
     </row>
-    <row r="499" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A499" s="1">
         <v>498</v>
       </c>
     </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A500" s="1">
         <v>499</v>
       </c>
     </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A501" s="1">
         <v>500</v>
       </c>
     </row>
-    <row r="502" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A502" s="1">
         <v>501</v>
       </c>
     </row>
-    <row r="503" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A503" s="1">
         <v>502</v>
       </c>
     </row>
-    <row r="504" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A504" s="1">
         <v>503</v>
       </c>
     </row>
-    <row r="505" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A505" s="1">
         <v>504</v>
       </c>
     </row>
-    <row r="506" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A506" s="1">
         <v>505</v>
       </c>
     </row>
-    <row r="507" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A507" s="1">
         <v>506</v>
       </c>
     </row>
-    <row r="508" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A508" s="1">
         <v>507</v>
       </c>
     </row>
-    <row r="509" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A509" s="1">
         <v>508</v>
       </c>
     </row>
-    <row r="510" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A510" s="1">
         <v>509</v>
       </c>
     </row>
-    <row r="511" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A511" s="1">
         <v>510</v>
       </c>
     </row>
-    <row r="512" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A512" s="1">
         <v>511</v>
       </c>
     </row>
-    <row r="513" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A513" s="1">
         <v>512</v>
       </c>
     </row>
-    <row r="514" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A514" s="1">
         <v>513</v>
       </c>
     </row>
-    <row r="515" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A515" s="1">
         <v>514</v>
       </c>
     </row>
-    <row r="516" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A516" s="1">
         <v>515</v>
       </c>
     </row>
-    <row r="517" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A517" s="1">
         <v>516</v>
       </c>
     </row>
-    <row r="518" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A518" s="1">
         <v>517</v>
       </c>
     </row>
-    <row r="519" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A519" s="1">
         <v>518</v>
       </c>
     </row>
-    <row r="520" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A520" s="1">
         <v>519</v>
       </c>
     </row>
-    <row r="521" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A521" s="1">
         <v>520</v>
       </c>
     </row>
-    <row r="522" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A522" s="1">
         <v>521</v>
       </c>
     </row>
-    <row r="523" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A523" s="1">
         <v>522</v>
       </c>
     </row>
-    <row r="524" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A524" s="1">
         <v>523</v>
       </c>
     </row>
-    <row r="525" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A525" s="1">
         <v>524</v>
       </c>
     </row>
-    <row r="526" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A526" s="1">
         <v>525</v>
       </c>
     </row>
-    <row r="527" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A527" s="1">
         <v>526</v>
       </c>
     </row>
-    <row r="528" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A528" s="1">
         <v>527</v>
       </c>
     </row>
-    <row r="529" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A529" s="1">
         <v>528</v>
       </c>
     </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A530" s="1">
         <v>529</v>
       </c>
     </row>
-    <row r="531" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A531" s="1">
         <v>530</v>
       </c>
     </row>
-    <row r="532" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A532" s="1">
         <v>531</v>
       </c>
     </row>
-    <row r="533" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A533" s="1">
         <v>532</v>
       </c>
     </row>
-    <row r="534" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A534" s="1">
         <v>533</v>
       </c>
     </row>
-    <row r="535" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A535" s="1">
         <v>534</v>
       </c>

</xml_diff>